<commit_message>
update: post-abs, sept 21-24 poll
</commit_message>
<xml_diff>
--- a/data-election-comparison/pres_vote_1988_16_65plus_senior_voters.xlsx
+++ b/data-election-comparison/pres_vote_1988_16_65plus_senior_voters.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janzilinsky/Documents/elections-and-voting/data-election-comparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225EA5D7-B67C-EE45-9E7F-7044B54EE8C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DA957B-F7AE-A04E-B087-A23D287DE06E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37240" yWindow="3840" windowWidth="28040" windowHeight="17040" xr2:uid="{74D28759-445F-BA4E-A93E-F6958861A85C}"/>
+    <workbookView xWindow="35840" yWindow="860" windowWidth="28800" windowHeight="17540" xr2:uid="{74D28759-445F-BA4E-A93E-F6958861A85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>year</t>
   </si>
@@ -48,16 +48,28 @@
     <t>rep_vote_margin_65plus</t>
   </si>
   <si>
-    <t>Washington Post-ABC (March 2020)</t>
-  </si>
-  <si>
-    <t>Pew (Summer 2020)</t>
-  </si>
-  <si>
-    <t>NYT/Siena (June 2020)</t>
-  </si>
-  <si>
-    <t>Marist (Sept. 2020)</t>
+    <t>The Economist/YouGov</t>
+  </si>
+  <si>
+    <t>WaPo-ABC (March)</t>
+  </si>
+  <si>
+    <t>Pew (Summer)</t>
+  </si>
+  <si>
+    <t>NYT/Siena (June)</t>
+  </si>
+  <si>
+    <t>Marist (Sept.)</t>
+  </si>
+  <si>
+    <t>Quinnipiac (July)</t>
+  </si>
+  <si>
+    <t>Emerson Coll. (July)</t>
+  </si>
+  <si>
+    <t>Nationscape (Apr.-June)</t>
   </si>
 </sst>
 </file>
@@ -415,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A149BB-9AAA-7B40-9E32-10B1682A5D26}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -448,7 +460,7 @@
         <v>-14</v>
       </c>
       <c r="D2">
-        <f>-C2</f>
+        <f t="shared" ref="D2:D10" si="0">-C2</f>
         <v>14</v>
       </c>
     </row>
@@ -463,7 +475,7 @@
         <v>-8</v>
       </c>
       <c r="D3">
-        <f>-C3</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -478,7 +490,7 @@
         <v>-8</v>
       </c>
       <c r="D4">
-        <f>-C4</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -493,7 +505,7 @@
         <v>-7</v>
       </c>
       <c r="D5">
-        <f>-C5</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -508,7 +520,7 @@
         <v>-12</v>
       </c>
       <c r="D6">
-        <f>-C6</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
@@ -523,7 +535,7 @@
         <v>-8</v>
       </c>
       <c r="D7">
-        <f>-C7</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -538,7 +550,7 @@
         <v>-12</v>
       </c>
       <c r="D8">
-        <f>-C8</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
@@ -553,7 +565,7 @@
         <v>-12</v>
       </c>
       <c r="D9">
-        <f>-C9</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
@@ -568,143 +580,203 @@
         <v>-14</v>
       </c>
       <c r="D10">
-        <f>-C10</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
-        <v>2020</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>7</v>
+        <v>2004</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>15</v>
+        <f>-D11</f>
+        <v>-5</v>
       </c>
       <c r="D11">
-        <f>-C11</f>
-        <v>-15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
-        <v>2020</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>8</v>
+        <v>2000</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
       </c>
       <c r="C12">
-        <v>-6</v>
+        <f>-D12</f>
+        <v>4</v>
       </c>
       <c r="D12">
-        <f>-C12</f>
-        <v>6</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13">
-        <v>2020</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>1996</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <f>-D13</f>
+        <v>6</v>
       </c>
       <c r="D13">
-        <f>-C13</f>
-        <v>-2</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14">
-        <v>2020</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>10</v>
+        <v>1992</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
       </c>
       <c r="C14">
-        <v>6</v>
+        <f>-D14</f>
+        <v>11</v>
       </c>
       <c r="D14">
-        <f>-C14</f>
-        <v>-6</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15">
-        <v>2004</v>
+        <v>1988</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
       </c>
       <c r="C15">
         <f>-D15</f>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16">
-        <v>2000</v>
-      </c>
-      <c r="B16" t="s">
-        <v>4</v>
+        <v>2020</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C16">
-        <f>-D16</f>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D16">
-        <v>-4</v>
+        <f>-C16</f>
+        <v>-15</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17">
-        <v>1996</v>
-      </c>
-      <c r="B17" t="s">
-        <v>4</v>
+        <v>2020</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C17">
-        <f>-D17</f>
+        <v>-6</v>
+      </c>
+      <c r="D17">
+        <f>-C17</f>
         <v>6</v>
-      </c>
-      <c r="D17">
-        <v>-6</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18">
-        <v>1992</v>
-      </c>
-      <c r="B18" t="s">
-        <v>4</v>
+        <v>2020</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C18">
-        <f>-D18</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D18">
-        <v>-11</v>
+        <f>-C18</f>
+        <v>-2</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19">
-        <v>1988</v>
-      </c>
-      <c r="B19" t="s">
-        <v>4</v>
+        <v>2020</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C19">
-        <f>-D19</f>
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <f>-C19</f>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>2020</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <v>14</v>
+      </c>
+      <c r="D20">
+        <f>-C20</f>
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>2020</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21">
+        <v>-20</v>
+      </c>
+      <c r="D21">
+        <f>-C21</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>2020</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <f>-C22</f>
         <v>-2</v>
       </c>
-      <c r="D19">
-        <v>2</v>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>2020</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23">
+        <v>7.9</v>
+      </c>
+      <c r="D23">
+        <f>-C23</f>
+        <v>-7.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>